<commit_message>
everything works (i hope)
</commit_message>
<xml_diff>
--- a/addresses.xlsx
+++ b/addresses.xlsx
@@ -16,12 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t>LastName1</t>
+  </si>
+  <si>
+    <t>FirstName1</t>
+  </si>
+  <si>
+    <t>LastName2</t>
+  </si>
+  <si>
+    <t>FirstName2</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
   </si>
   <si>
     <t>City</t>
@@ -33,7 +45,13 @@
     <t>Zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Olivia Chen</t>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>Olivia</t>
   </si>
   <si>
     <t xml:space="preserve">123 Maple St</t>
@@ -45,7 +63,13 @@
     <t>CA</t>
   </si>
   <si>
-    <t xml:space="preserve">Benjamin Carter</t>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Sarah</t>
   </si>
   <si>
     <t xml:space="preserve">456 Oak Ave</t>
@@ -57,19 +81,34 @@
     <t>TX</t>
   </si>
   <si>
-    <t xml:space="preserve">Sophia Rodriguez</t>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Sophia</t>
   </si>
   <si>
     <t xml:space="preserve">789 Pine Ln</t>
   </si>
   <si>
+    <t xml:space="preserve">PO Box 200</t>
+  </si>
+  <si>
     <t>Springfield</t>
   </si>
   <si>
     <t>IL</t>
   </si>
   <si>
-    <t xml:space="preserve">Liam Goldberg</t>
+    <t>Goldberg</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Miller</t>
   </si>
   <si>
     <t xml:space="preserve">101 Cedar Ct</t>
@@ -81,7 +120,10 @@
     <t>OR</t>
   </si>
   <si>
-    <t xml:space="preserve">Ava Nguyen</t>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Ava</t>
   </si>
   <si>
     <t xml:space="preserve">212 Elm Dr</t>
@@ -93,7 +135,13 @@
     <t>FL</t>
   </si>
   <si>
-    <t xml:space="preserve">Noah Patel</t>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>Noah</t>
   </si>
   <si>
     <t xml:space="preserve">333 Birch Rd</t>
@@ -105,7 +153,10 @@
     <t>CO</t>
   </si>
   <si>
-    <t xml:space="preserve">Isabella Martinez</t>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Isabella</t>
   </si>
   <si>
     <t xml:space="preserve">444 Spruce Way</t>
@@ -117,7 +168,10 @@
     <t>WA</t>
   </si>
   <si>
-    <t xml:space="preserve">Lucas Williams</t>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Lucas</t>
   </si>
   <si>
     <t xml:space="preserve">555 Willow Creek</t>
@@ -129,7 +183,10 @@
     <t>MA</t>
   </si>
   <si>
-    <t xml:space="preserve">Mia Kim</t>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Mia</t>
   </si>
   <si>
     <t xml:space="preserve">667 Maple St</t>
@@ -139,120 +196,6 @@
   </si>
   <si>
     <t>CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jackson Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">778 Oak Ave</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amelia Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">889 Pine Ln</t>
-  </si>
-  <si>
-    <t>Springfield</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aiden Garcia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">990 Cedar Ct</t>
-  </si>
-  <si>
-    <t>Portland</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harper Miller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111 Elm Dr</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elijah Davis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222 Birch Rd</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evelyn Wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">334 Spruce Way</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logan Moore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">445 Willow Creek</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abigail Taylor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">556 Maple St</t>
-  </si>
-  <si>
-    <t>Sunnyvale</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mason Anderson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667 Oak Ave</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>testing</t>
   </si>
 </sst>
 </file>
@@ -287,7 +230,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -748,350 +692,317 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="15.76171875"/>
+    <col customWidth="1" min="1" max="4" width="15.57421875"/>
+    <col bestFit="1" min="5" max="5" width="15.34375"/>
+    <col min="6" max="6" width="15.34375"/>
   </cols>
   <sheetData>
-    <row r="2" ht="14.25">
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>94086</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>94086</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>78701</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>78701</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4">
+        <v>62704</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>62704</v>
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5">
+        <v>97209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>97209</v>
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6">
+        <v>33132</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <v>33132</v>
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7">
+        <v>80202</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8">
-        <v>80202</v>
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8">
+        <v>98101</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9">
-        <v>98101</v>
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9">
+        <v>2110</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10">
-        <v>2110</v>
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10">
+        <v>94086</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11">
-        <v>94086</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12">
-        <v>78701</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13">
-        <v>62704</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14">
-        <v>97209</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15">
-        <v>33132</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16">
-        <v>80202</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17">
-        <v>98101</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18">
-        <v>2110</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19">
-        <v>94086</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20">
-        <v>68555</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="D26" t="s">
-        <v>78</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="F22" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>